<commit_message>
commit after error fixes and running solution for Question 1. EOD work for thursday...
</commit_message>
<xml_diff>
--- a/data/Emirates.xlsx
+++ b/data/Emirates.xlsx
@@ -18,10 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
-  <si>
-    <t>UserName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -53,181 +50,217 @@
     <t>CHROME</t>
   </si>
   <si>
+    <t>rHub</t>
+  </si>
+  <si>
+    <t>rPort</t>
+  </si>
+  <si>
+    <t>rPlatform</t>
+  </si>
+  <si>
+    <t>rBrowser</t>
+  </si>
+  <si>
+    <t>PlatformName</t>
+  </si>
+  <si>
+    <t>PlatformVersion</t>
+  </si>
+  <si>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>udid</t>
+  </si>
+  <si>
+    <t>AppPackage</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>AppActivity</t>
+  </si>
+  <si>
+    <t>DeviceOrientation</t>
+  </si>
+  <si>
+    <t>AppiumVersion</t>
+  </si>
+  <si>
+    <t>127.0.0.1:4723</t>
+  </si>
+  <si>
+    <t>portNumber</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>8.0.1</t>
+  </si>
+  <si>
+    <t>OnePlus 5</t>
+  </si>
+  <si>
+    <t># Home Page Objects</t>
+  </si>
+  <si>
+    <t>#Page.ObjectName.Locator</t>
+  </si>
+  <si>
+    <t>value given by developer</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Home.Title</t>
+  </si>
+  <si>
+    <t>4444</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Search Emirates Flights</t>
+  </si>
+  <si>
+    <t>Search Flights for the specified Departure and Arival Destinations for both Oneway and Return types</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>https://www.emirates.com/ae/english/</t>
+  </si>
+  <si>
+    <t>Emirates flights – Book a flight, browse our flight offers and explore the Emirates Experience</t>
+  </si>
+  <si>
+    <t>(//*[@name='Departure airport'])[1]</t>
+  </si>
+  <si>
+    <t>(//*[@name='Arrival airport'])[1]</t>
+  </si>
+  <si>
+    <t>//*[@class='checkbox one-way']/input</t>
+  </si>
+  <si>
+    <t>(//button[@type='submit'])[1]</t>
+  </si>
+  <si>
+    <t>#Search Result Page Objects</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-OB"]/text()</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-IB"]/text()</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-OB"]/text()/following::div[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-IB"]/text()/following::div[1]</t>
+  </si>
+  <si>
+    <t>Result.Title</t>
+  </si>
+  <si>
+    <t>Search results | Make a booking | Emirates</t>
+  </si>
+  <si>
+    <t>(//*[@class='ts-fbr-flight-list__body'])[1]/div</t>
+  </si>
+  <si>
+    <t>(//*[@class='ts-fbr-flight-list__body'])[2]/div</t>
+  </si>
+  <si>
+    <t>(//*[@class='location__list']/li)[1]</t>
+  </si>
+  <si>
+    <t>Home.Departure.Xpath</t>
+  </si>
+  <si>
+    <t>Home.DepartureSelect.Xpath</t>
+  </si>
+  <si>
+    <t>Home.Arrival.Xpath</t>
+  </si>
+  <si>
+    <t>Home.ArrivalSelect.Xpath</t>
+  </si>
+  <si>
+    <t>Home.Oneway.Xpath</t>
+  </si>
+  <si>
+    <t>Home.DepartureDate.Xpath</t>
+  </si>
+  <si>
+    <t>Home.ArrivalDate.Xpath</t>
+  </si>
+  <si>
+    <t>Home.SearchButton.Xpath</t>
+  </si>
+  <si>
+    <t>Result.OutBound.Xpath</t>
+  </si>
+  <si>
+    <t>Result.InBound.Xpath</t>
+  </si>
+  <si>
+    <t>Result.ObDate.Xpath</t>
+  </si>
+  <si>
+    <t>Result.IbDate.Xapth</t>
+  </si>
+  <si>
+    <t>Result.ObList.Xapth</t>
+  </si>
+  <si>
+    <t>Reuslt.IbList.Xpath</t>
+  </si>
+  <si>
+    <t>(//a[@data-string='"+arrivalDate"+'])[1]</t>
+  </si>
+  <si>
+    <t>(//a[@data-string='"+"departureDate"+'])[1]</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>DepartureDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepartureLocation </t>
+  </si>
+  <si>
+    <t>ArrivalLocation</t>
+  </si>
+  <si>
+    <t>28092019</t>
+  </si>
+  <si>
+    <t>27102019</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>ReturnDate</t>
+  </si>
+  <si>
     <t>chrome</t>
   </si>
   <si>
-    <t>rHub</t>
-  </si>
-  <si>
-    <t>rPort</t>
-  </si>
-  <si>
-    <t>rPlatform</t>
-  </si>
-  <si>
-    <t>rBrowser</t>
-  </si>
-  <si>
-    <t>PlatformName</t>
-  </si>
-  <si>
-    <t>PlatformVersion</t>
-  </si>
-  <si>
-    <t>DeviceName</t>
-  </si>
-  <si>
-    <t>udid</t>
-  </si>
-  <si>
-    <t>AppPackage</t>
-  </si>
-  <si>
-    <t>App</t>
-  </si>
-  <si>
-    <t>AppActivity</t>
-  </si>
-  <si>
-    <t>DeviceOrientation</t>
-  </si>
-  <si>
-    <t>AppiumVersion</t>
-  </si>
-  <si>
-    <t>127.0.0.1:4723</t>
-  </si>
-  <si>
-    <t>portNumber</t>
-  </si>
-  <si>
-    <t>Android</t>
-  </si>
-  <si>
-    <t>8.0.1</t>
-  </si>
-  <si>
-    <t>OnePlus 5</t>
-  </si>
-  <si>
-    <t># Home Page Objects</t>
-  </si>
-  <si>
-    <t>#Page.ObjectName.Locator</t>
-  </si>
-  <si>
-    <t>value given by developer</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>Home.Title</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>4444</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Search Emirates Flights</t>
-  </si>
-  <si>
-    <t>Search Flights for the specified Departure and Arival Destinations for both Oneway and Return types</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>https://www.emirates.com/ae/english/</t>
-  </si>
-  <si>
-    <t>Emirates flights – Book a flight, browse our flight offers and explore the Emirates Experience</t>
-  </si>
-  <si>
-    <t>Home.Departure</t>
-  </si>
-  <si>
-    <t>(//*[@name='Departure airport'])[1]</t>
-  </si>
-  <si>
-    <t>(//*[@name='Arrival airport'])[1]</t>
-  </si>
-  <si>
-    <t>Home.Arrival</t>
-  </si>
-  <si>
-    <t>Home.Oneway</t>
-  </si>
-  <si>
-    <t>//*[@class='checkbox one-way']/input</t>
-  </si>
-  <si>
-    <t>(//a[@data-string='2882019'])[1]</t>
-  </si>
-  <si>
-    <t>Home.DepartureDate</t>
-  </si>
-  <si>
-    <t>Home.ArrivalDate</t>
-  </si>
-  <si>
-    <t>(//a[@data-string='2792019'])[1]</t>
-  </si>
-  <si>
-    <t>(//button[@type='submit'])[1]</t>
-  </si>
-  <si>
-    <t>Home.SearchButton</t>
-  </si>
-  <si>
-    <t>#Search Result Page Objects</t>
-  </si>
-  <si>
-    <t>Result.OutBound</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-OB"]/text()</t>
-  </si>
-  <si>
-    <t>Result.InBound</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-IB"]/text()</t>
-  </si>
-  <si>
-    <t>Result.ObDate</t>
-  </si>
-  <si>
-    <t>Result.IbDate</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-OB"]/text()/following::div[1]</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-IB"]/text()/following::div[1]</t>
-  </si>
-  <si>
-    <t>Result.Title</t>
-  </si>
-  <si>
-    <t>Search results | Make a booking | Emirates</t>
-  </si>
-  <si>
-    <t>Result.ObList</t>
-  </si>
-  <si>
-    <t>(//*[@class='ts-fbr-flight-list__body'])[1]/div</t>
-  </si>
-  <si>
-    <t>Reuslt.IbList</t>
-  </si>
-  <si>
-    <t>(//*[@class='ts-fbr-flight-list__body'])[2]/div</t>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>(//*[@class='location__list']/li[1])[4]/div</t>
   </si>
 </sst>
 </file>
@@ -571,7 +604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -581,19 +614,38 @@
   <cols>
     <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2"/>
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -603,66 +655,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="92" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="45.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -686,34 +749,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -737,90 +800,90 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -830,162 +893,183 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A8" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A8" r:id="rId4"/>
+    <hyperlink ref="A9" r:id="rId5"/>
+    <hyperlink ref="A10" r:id="rId6"/>
+    <hyperlink ref="A11" r:id="rId7"/>
+    <hyperlink ref="A5" r:id="rId8"/>
+    <hyperlink ref="A7" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completely working solution for the Question 1. Result with screenshots are in latest test run reports.
</commit_message>
<xml_diff>
--- a/data/Emirates.xlsx
+++ b/data/Emirates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -155,18 +155,6 @@
     <t>#Search Result Page Objects</t>
   </si>
   <si>
-    <t>//*[@id="leg-OB"]/text()</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-IB"]/text()</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-OB"]/text()/following::div[1]</t>
-  </si>
-  <si>
-    <t>//*[@id="leg-IB"]/text()/following::div[1]</t>
-  </si>
-  <si>
     <t>Result.Title</t>
   </si>
   <si>
@@ -200,9 +188,6 @@
     <t>Home.DepartureDate.Xpath</t>
   </si>
   <si>
-    <t>Home.ArrivalDate.Xpath</t>
-  </si>
-  <si>
     <t>Home.SearchButton.Xpath</t>
   </si>
   <si>
@@ -224,36 +209,18 @@
     <t>Reuslt.IbList.Xpath</t>
   </si>
   <si>
-    <t>(//a[@data-string='"+arrivalDate"+'])[1]</t>
-  </si>
-  <si>
-    <t>(//a[@data-string='"+"departureDate"+'])[1]</t>
-  </si>
-  <si>
     <t>Chennai</t>
   </si>
   <si>
-    <t>DepartureDate</t>
-  </si>
-  <si>
     <t xml:space="preserve">DepartureLocation </t>
   </si>
   <si>
     <t>ArrivalLocation</t>
   </si>
   <si>
-    <t>28092019</t>
-  </si>
-  <si>
-    <t>27102019</t>
-  </si>
-  <si>
     <t>values</t>
   </si>
   <si>
-    <t>ReturnDate</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -261,6 +228,27 @@
   </si>
   <si>
     <t>(//*[@class='location__list']/li[1])[4]/div</t>
+  </si>
+  <si>
+    <t>(//a[@data-string='2882019'])[1]</t>
+  </si>
+  <si>
+    <t>(//a[@data-string='2792019'])[1]</t>
+  </si>
+  <si>
+    <t>Home.ReturnDate.Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-OB"]</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-IB"]</t>
+  </si>
+  <si>
+    <t>//*[@id="leg-OB"]/following::div[1]</t>
+  </si>
+  <si>
+    <t>(//*[@id="leg-IB"]/following::div)[1]</t>
   </si>
 </sst>
 </file>
@@ -604,47 +592,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -896,7 +870,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -931,7 +905,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -939,15 +913,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -955,15 +929,15 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -971,23 +945,23 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -998,63 +972,63 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solution for Question 2 added. Solution has been committed...
</commit_message>
<xml_diff>
--- a/data/Emirates.xlsx
+++ b/data/Emirates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Android</t>
   </si>
   <si>
-    <t>8.0.1</t>
-  </si>
-  <si>
     <t>OnePlus 5</t>
   </si>
   <si>
@@ -249,6 +246,21 @@
   </si>
   <si>
     <t>(//*[@id="leg-IB"]/following::div)[1]</t>
+  </si>
+  <si>
+    <t>a9304017</t>
+  </si>
+  <si>
+    <t>1.14.2</t>
+  </si>
+  <si>
+    <t>Portrait</t>
+  </si>
+  <si>
+    <t>com.emirates.ek.android</t>
+  </si>
+  <si>
+    <t>./apk/com.emirates.ek.android.apk</t>
   </si>
 </sst>
 </file>
@@ -607,18 +619,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -656,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -664,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -672,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -688,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -734,7 +746,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -762,14 +774,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -792,8 +804,8 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
+      <c r="B3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -801,7 +813,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -809,7 +821,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -817,7 +829,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -825,39 +837,39 @@
         <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>34</v>
+      <c r="B8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
+      <c r="B9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>34</v>
+      <c r="B10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>34</v>
+      <c r="B11" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -869,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -881,154 +893,154 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>